<commit_message>
basic module added (#8)
</commit_message>
<xml_diff>
--- a/data/inventory.xlsx
+++ b/data/inventory.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,72 +446,74 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
+          <t>category</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>suppliers</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>customers</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
           <t>quantity</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>price</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>created_at</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>updated_at</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>category</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>supplier</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>reorder_point</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>01f55631-94c1-4719-bf52-94814bfbde8c</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>hammer</t>
-        </is>
-      </c>
-      <c r="C2" t="n">
-        <v>8</v>
-      </c>
-      <c r="D2" t="n">
-        <v>78</v>
+          <t>5fbe7df6-340c-460c-b064-3dbf08aa63d7</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>cee738ea-c625-4c80-add1-b875a50aa499</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>["2f0e4354-8965-4cc4-8b57-b685d58039c0"]</t>
+        </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>2024-11-09T20:16:23.455512</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>2024-11-09T20:16:23.455512</t>
-        </is>
+          <t>["e664bdf5-f208-4757-9be2-425c3dc3b6d6"]</t>
+        </is>
+      </c>
+      <c r="F2" t="n">
+        <v>1</v>
       </c>
       <c r="G2" t="n">
-        <v>0</v>
-      </c>
-      <c r="H2" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>2024-11-17T12:26:27.664712</t>
+        </is>
       </c>
       <c r="I2" t="n">
         <v>0</v>
@@ -520,177 +522,39 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>ead516ec-d0bd-4426-90b5-c7e488d98521</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>hammer</t>
-        </is>
-      </c>
-      <c r="C3" t="n">
-        <v>10</v>
-      </c>
-      <c r="D3" t="n">
-        <v>78</v>
+          <t>0c291ffb-a8d8-47fb-8cf9-235fe6a54b62</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>cee738ea-c625-4c80-add1-b875a50aa499</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>["ee77754b-f795-469d-a40d-998282b919e6", "2f0e4354-8965-4cc4-8b57-b685d58039c0"]</t>
+        </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>2024-11-09T20:17:55.632723</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>2024-11-09T20:17:55.632723</t>
-        </is>
+          <t>["e664bdf5-f208-4757-9be2-425c3dc3b6d6"]</t>
+        </is>
+      </c>
+      <c r="F3" t="n">
+        <v>123</v>
       </c>
       <c r="G3" t="n">
-        <v>0</v>
-      </c>
-      <c r="H3" t="n">
-        <v>0</v>
+        <v>1234</v>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>2024-11-17T12:32:05.218225</t>
+        </is>
       </c>
       <c r="I3" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>1fd15b25-ce16-4245-bc59-88c1df216248</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>hammer</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
-        <v>10</v>
-      </c>
-      <c r="D4" t="n">
-        <v>78</v>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>2024-11-09T20:18:18.411197</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>2024-11-09T20:18:18.411197</t>
-        </is>
-      </c>
-      <c r="G4" t="n">
-        <v>0</v>
-      </c>
-      <c r="H4" t="n">
-        <v>0</v>
-      </c>
-      <c r="I4" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>88521977-ae8e-4a6b-b575-0aa4a9fdef44</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>hammer</t>
-        </is>
-      </c>
-      <c r="C5" t="n">
-        <v>10</v>
-      </c>
-      <c r="D5" t="n">
-        <v>78</v>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>2024-11-09T20:18:40.128526</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>2024-11-09T20:18:40.128526</t>
-        </is>
-      </c>
-      <c r="G5" t="n">
-        <v>0</v>
-      </c>
-      <c r="H5" t="n">
-        <v>0</v>
-      </c>
-      <c r="I5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>5a7c37df-617a-45b3-a13d-c82c3e4c3fa6</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Test1</t>
-        </is>
-      </c>
-      <c r="C6" t="n">
-        <v>5</v>
-      </c>
-      <c r="D6" t="n">
-        <v>10</v>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>2024-11-09T23:34:56.291016</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>2024-11-09T23:34:56.291016</t>
-        </is>
-      </c>
-      <c r="G6" t="n">
-        <v>0</v>
-      </c>
-      <c r="H6" t="n">
-        <v>0</v>
-      </c>
-      <c r="I6" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>905c9916-1d42-4387-b8f3-1545981ef9a2</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>Hasnain Lakhani</t>
-        </is>
-      </c>
-      <c r="C7" t="n">
-        <v>1</v>
-      </c>
-      <c r="D7" t="n">
-        <v>2</v>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>2024-11-15T10:49:48.030131</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr"/>
-      <c r="G7" t="inlineStr"/>
-      <c r="H7" t="inlineStr"/>
-      <c r="I7" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>